<commit_message>
try to revise and resubmit
</commit_message>
<xml_diff>
--- a/GAMS/AQ_LEWIE_InputSheet.xlsx
+++ b/GAMS/AQ_LEWIE_InputSheet.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Docs\Myanmar\AquaAgri\Analysis\AquaLEWIE_github\GAMS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="21150" windowHeight="6260" tabRatio="736" activeTab="5"/>
   </bookViews>
@@ -23,7 +18,7 @@
     <sheet name="Endow" sheetId="24" r:id="rId9"/>
     <sheet name="Index_div" sheetId="15" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -62,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="176">
   <si>
     <t>Variable</t>
   </si>
@@ -595,7 +590,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="9">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -607,7 +602,7 @@
     <numFmt numFmtId="170" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="171" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -686,7 +681,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79995117038483843"/>
+        <fgColor theme="3" tint="0.79995117038484"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -698,25 +693,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
+        <fgColor theme="3" tint="0.39997558519242"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59996337778862885"/>
+        <fgColor theme="8" tint="0.59996337778863"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59996337778862885"/>
+        <fgColor theme="6" tint="0.59996337778863"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.39997558519242"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -728,19 +723,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59996337778862885"/>
+        <fgColor theme="6" tint="0.59996337778863"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79995117038483843"/>
+        <fgColor theme="3" tint="0.79995117038484"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79995117038483843"/>
+        <fgColor theme="6" tint="0.79995117038484"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -752,37 +747,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.24994659260841701"/>
+        <fgColor theme="0" tint="-0.24994659260842"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407453"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.39997558519242"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59996337778862885"/>
+        <fgColor theme="7" tint="0.59996337778863"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59996337778862885"/>
+        <fgColor theme="9" tint="0.59996337778863"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.39997558519242"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -794,49 +789,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59996337778862885"/>
+        <fgColor theme="8" tint="0.59996337778863"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59996337778862885"/>
+        <fgColor theme="9" tint="0.59996337778863"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79995117038483843"/>
+        <fgColor theme="4" tint="0.79995117038484"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.39997558519242"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79995117038483843"/>
+        <fgColor theme="3" tint="0.79995117038484"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59996337778862885"/>
+        <fgColor theme="6" tint="0.59996337778863"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79995117038483843"/>
+        <fgColor theme="3" tint="0.79995117038484"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59996337778862885"/>
+        <fgColor theme="9" tint="0.59996337778863"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1021,578 +1016,578 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="326">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyAlignment="true"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true" applyAlignment="true"/>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="14" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="10" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="10" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="15" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true"/>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="14" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="15" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="12" borderId="14" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="12" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="12" borderId="15" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="14" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="15" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="14" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="14" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="12" borderId="8" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="12" borderId="9" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="12" borderId="10" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="8" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="9" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="13" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="13" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="13" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="9" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="1" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="13" borderId="8" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="13" borderId="9" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="13" borderId="10" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="11" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="11" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="11" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="11" borderId="14" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="11" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="11" borderId="15" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="14" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="14" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="8" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="14" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="14" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="10" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="15" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="15" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="14" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="171" fontId="0" fillId="3" borderId="14" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="12" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="14" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="14" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="15" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="12" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="1" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="18" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="18" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="18" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="18" borderId="14" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="171" fontId="0" fillId="18" borderId="14" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="15" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="18" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="18" borderId="15" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="12" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="1" fontId="0" fillId="19" borderId="1" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="19" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="19" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="19" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="19" borderId="14" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="171" fontId="0" fillId="19" borderId="14" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="15" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="19" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="19" borderId="15" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="16" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="15" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="12" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="14" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="3" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="15" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="16" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="15" borderId="14" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="15" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="15" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="16" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="15" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="15" borderId="15" xfId="1" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="16" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="15" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="15" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="15" borderId="14" xfId="1" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="15" borderId="15" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="15" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="15" borderId="15" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="17" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="18" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="17" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="18" borderId="14" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="18" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="18" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="17" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="18" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="18" borderId="15" xfId="1" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="17" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="19" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="20" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="19" borderId="14" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="19" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="19" borderId="14" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="19" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="19" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="19" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="19" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="19" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="19" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="19" borderId="15" xfId="1" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="19" borderId="15" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="20" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="20" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="21" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="21" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="9" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="9" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="25" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="24" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="24" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="25" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="25" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="28" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="24" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="24" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="5" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="6" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="12" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="13" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="14" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="14" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="3" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="11" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="15" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="25" borderId="15" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true"/>
+    <xf numFmtId="164" fontId="0" fillId="28" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="29" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="3" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="2" fontId="0" fillId="29" borderId="10" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="2" fontId="0" fillId="20" borderId="9" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="20" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="20" borderId="2" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="20" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="20" borderId="13" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="20" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="20" borderId="13" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="20" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="20" borderId="11" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="29" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="29" borderId="13" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="29" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="29" borderId="13" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="29" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="29" borderId="11" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="29" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="29" borderId="11" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="20" borderId="8" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="29" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="29" borderId="8" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="20" borderId="8" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="20" borderId="9" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="29" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="29" borderId="8" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="29" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="29" borderId="9" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="29" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="29" borderId="10" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="20" borderId="10" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="20" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="20" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="9" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="10" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="10" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="9" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="10" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="9" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="10" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1608,14 +1603,6 @@
       <color rgb="FFFFFF99"/>
     </mruColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1939,21 +1926,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="2" width="8.81640625" style="2"/>
-    <col min="3" max="3" width="19" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19" style="2" customWidth="true"/>
     <col min="4" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -1967,7 +1954,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="D2" s="2" t="s">
         <v>32</v>
       </c>
@@ -1975,7 +1962,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3">
       <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
@@ -1989,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
@@ -2003,7 +1990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -2017,7 +2004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -2031,7 +2018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
@@ -2045,7 +2032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8">
       <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
@@ -2068,21 +2055,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="21.453125" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" customWidth="true"/>
+    <col min="4" max="4" width="11.26953125" customWidth="true"/>
+    <col min="5" max="5" width="12" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -2097,7 +2084,7 @@
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2108,7 +2095,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3">
       <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
@@ -2123,7 +2110,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
@@ -2138,7 +2125,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -2153,7 +2140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -2168,7 +2155,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
@@ -2183,7 +2170,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8">
       <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
@@ -2206,21 +2193,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.26953125" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" customWidth="true"/>
+    <col min="2" max="2" width="30.26953125" customWidth="true"/>
+    <col min="3" max="3" width="29" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="A1" s="3" t="s">
         <v>43</v>
       </c>
@@ -2231,7 +2218,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -2242,7 +2229,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -2253,7 +2240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -2264,7 +2251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -2275,7 +2262,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6">
       <c r="A6" s="225" t="s">
         <v>26</v>
       </c>
@@ -2286,7 +2273,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7">
       <c r="A7" s="9" t="s">
         <v>85</v>
       </c>
@@ -2297,7 +2284,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8">
       <c r="A8" s="9" t="s">
         <v>86</v>
       </c>
@@ -2308,7 +2295,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9">
       <c r="A9" s="9" t="s">
         <v>169</v>
       </c>
@@ -2319,7 +2306,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10">
       <c r="A10" s="9" t="s">
         <v>88</v>
       </c>
@@ -2330,7 +2317,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
@@ -2341,7 +2328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12">
       <c r="A12" s="9" t="s">
         <v>87</v>
       </c>
@@ -2352,7 +2339,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13">
       <c r="A13" s="226" t="s">
         <v>89</v>
       </c>
@@ -2363,7 +2350,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14">
       <c r="A14" s="222" t="s">
         <v>116</v>
       </c>
@@ -2374,7 +2361,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15">
       <c r="A15" s="222" t="s">
         <v>117</v>
       </c>
@@ -2385,7 +2372,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16">
       <c r="A16" s="9" t="s">
         <v>171</v>
       </c>
@@ -2396,7 +2383,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17">
       <c r="A17" s="222" t="s">
         <v>132</v>
       </c>
@@ -2405,7 +2392,7 @@
       </c>
       <c r="C17" s="222"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18">
       <c r="A18" s="222" t="s">
         <v>118</v>
       </c>
@@ -2413,13 +2400,13 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19">
       <c r="A19" s="223"/>
       <c r="B19" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20">
       <c r="A20" s="223"/>
       <c r="B20" s="223"/>
     </row>
@@ -2429,7 +2416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -2442,19 +2429,19 @@
       <selection pane="bottomRight" activeCell="J86" sqref="J86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" style="228" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" customWidth="1"/>
-    <col min="6" max="9" width="17.453125" style="113" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" style="120" customWidth="1"/>
-    <col min="11" max="11" width="17.453125" style="119" customWidth="1"/>
-    <col min="12" max="12" width="34.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" style="228" customWidth="true"/>
+    <col min="2" max="2" width="16.81640625" customWidth="true"/>
+    <col min="3" max="3" width="12" customWidth="true"/>
+    <col min="5" max="5" width="8.1796875" customWidth="true"/>
+    <col min="6" max="9" width="17.453125" style="113" customWidth="true"/>
+    <col min="10" max="10" width="17.453125" style="120" customWidth="true"/>
+    <col min="11" max="11" width="17.453125" style="119" customWidth="true"/>
+    <col min="12" max="12" width="34.453125" style="1" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2477,7 +2464,7 @@
       <c r="K1" s="250"/>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2493,7 +2480,7 @@
       <c r="J2" s="119"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2515,7 +2502,7 @@
       </c>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -2538,7 +2525,7 @@
       <c r="K4" s="224"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" ht="15" customHeight="true">
       <c r="A5" s="323" t="s">
         <v>140</v>
       </c>
@@ -2573,7 +2560,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" ht="15" customHeight="true">
       <c r="A6" s="324"/>
       <c r="B6" s="216" t="s">
         <v>133</v>
@@ -2606,7 +2593,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" ht="15" customHeight="true">
       <c r="A7" s="325"/>
       <c r="B7" s="216" t="s">
         <v>135</v>
@@ -2623,7 +2610,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" ht="15" customHeight="true">
       <c r="A8" s="320" t="s">
         <v>139</v>
       </c>
@@ -2642,7 +2629,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9">
       <c r="A9" s="321"/>
       <c r="B9" s="232" t="s">
         <v>46</v>
@@ -2675,7 +2662,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10">
       <c r="A10" s="321"/>
       <c r="B10" s="33" t="s">
         <v>124</v>
@@ -2708,7 +2695,7 @@
       <c r="K10" s="253"/>
       <c r="L10" s="28"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11">
       <c r="A11" s="321"/>
       <c r="B11" s="33" t="s">
         <v>124</v>
@@ -2741,7 +2728,7 @@
       <c r="K11" s="253"/>
       <c r="L11" s="28"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12">
       <c r="A12" s="321"/>
       <c r="B12" s="33" t="s">
         <v>124</v>
@@ -2774,7 +2761,7 @@
       <c r="K12" s="253"/>
       <c r="L12" s="28"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13">
       <c r="A13" s="321"/>
       <c r="B13" s="33" t="s">
         <v>124</v>
@@ -2807,7 +2794,7 @@
       <c r="K13" s="253"/>
       <c r="L13" s="28"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14">
       <c r="A14" s="321"/>
       <c r="B14" s="33" t="s">
         <v>124</v>
@@ -2840,7 +2827,7 @@
       <c r="K14" s="253"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15">
       <c r="A15" s="321"/>
       <c r="B15" s="33" t="s">
         <v>124</v>
@@ -2873,7 +2860,7 @@
       <c r="K15" s="253"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16">
       <c r="A16" s="321"/>
       <c r="B16" s="33" t="s">
         <v>124</v>
@@ -2906,7 +2893,7 @@
       <c r="K16" s="253"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17">
       <c r="A17" s="321"/>
       <c r="B17" s="50" t="s">
         <v>125</v>
@@ -2941,7 +2928,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18">
       <c r="A18" s="321"/>
       <c r="B18" s="50" t="s">
         <v>125</v>
@@ -2974,7 +2961,7 @@
       <c r="K18" s="255"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19">
       <c r="A19" s="321"/>
       <c r="B19" s="50" t="s">
         <v>125</v>
@@ -3007,7 +2994,7 @@
       <c r="K19" s="255"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20">
       <c r="A20" s="321"/>
       <c r="B20" s="50" t="s">
         <v>125</v>
@@ -3040,7 +3027,7 @@
       <c r="K20" s="255"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21">
       <c r="A21" s="321"/>
       <c r="B21" s="50" t="s">
         <v>125</v>
@@ -3073,7 +3060,7 @@
       <c r="K21" s="255"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22">
       <c r="A22" s="321"/>
       <c r="B22" s="50" t="s">
         <v>125</v>
@@ -3106,7 +3093,7 @@
       <c r="K22" s="255"/>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23">
       <c r="A23" s="321"/>
       <c r="B23" s="50" t="s">
         <v>125</v>
@@ -3139,7 +3126,7 @@
       <c r="K23" s="256"/>
       <c r="L23" s="4"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24">
       <c r="A24" s="321"/>
       <c r="B24" s="56" t="s">
         <v>126</v>
@@ -3159,7 +3146,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" ht="15" customHeight="true">
       <c r="A25" s="321"/>
       <c r="B25" s="56" t="s">
         <v>126</v>
@@ -3177,7 +3164,7 @@
       <c r="K25" s="258"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26">
       <c r="A26" s="321"/>
       <c r="B26" s="56" t="s">
         <v>126</v>
@@ -3194,7 +3181,7 @@
       <c r="J26" s="37"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27">
       <c r="A27" s="321"/>
       <c r="B27" s="56" t="s">
         <v>126</v>
@@ -3212,7 +3199,7 @@
       <c r="K27" s="259"/>
       <c r="L27" s="28"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28">
       <c r="A28" s="321"/>
       <c r="B28" s="56" t="s">
         <v>126</v>
@@ -3230,7 +3217,7 @@
       <c r="K28" s="259"/>
       <c r="L28" s="28"/>
     </row>
-    <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" ht="15" customHeight="true">
       <c r="A29" s="321"/>
       <c r="B29" s="56" t="s">
         <v>126</v>
@@ -3248,7 +3235,7 @@
       <c r="K29" s="259"/>
       <c r="L29" s="28"/>
     </row>
-    <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" ht="15" customHeight="true">
       <c r="A30" s="321"/>
       <c r="B30" s="56" t="s">
         <v>126</v>
@@ -3266,7 +3253,7 @@
       <c r="K30" s="260"/>
       <c r="L30" s="28"/>
     </row>
-    <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" ht="15" customHeight="true">
       <c r="A31" s="321"/>
       <c r="B31" s="34" t="s">
         <v>18</v>
@@ -3282,7 +3269,7 @@
       <c r="K31" s="260"/>
       <c r="L31" s="193"/>
     </row>
-    <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" ht="15" customHeight="true">
       <c r="A32" s="321"/>
       <c r="B32" s="34" t="s">
         <v>115</v>
@@ -3298,7 +3285,7 @@
       <c r="K32" s="260"/>
       <c r="L32" s="193"/>
     </row>
-    <row r="33" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" ht="15" customHeight="true">
       <c r="A33" s="321"/>
       <c r="B33" s="34" t="s">
         <v>19</v>
@@ -3314,7 +3301,7 @@
       <c r="K33" s="260"/>
       <c r="L33" s="193"/>
     </row>
-    <row r="34" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" ht="15" customHeight="true">
       <c r="A34" s="321"/>
       <c r="B34" s="34" t="s">
         <v>114</v>
@@ -3330,7 +3317,7 @@
       <c r="K34" s="260"/>
       <c r="L34" s="193"/>
     </row>
-    <row r="35" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" ht="15" customHeight="true">
       <c r="A35" s="321"/>
       <c r="B35" s="34" t="s">
         <v>130</v>
@@ -3346,7 +3333,7 @@
       <c r="K35" s="260"/>
       <c r="L35" s="193"/>
     </row>
-    <row r="36" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" ht="15" customHeight="true">
       <c r="A36" s="322"/>
       <c r="B36" s="34" t="s">
         <v>131</v>
@@ -3362,7 +3349,7 @@
       <c r="K36" s="260"/>
       <c r="L36" s="193"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="37">
       <c r="A37" s="311" t="s">
         <v>141</v>
       </c>
@@ -3390,7 +3377,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" s="3" customFormat="true">
       <c r="A38" s="312"/>
       <c r="B38" s="67" t="s">
         <v>129</v>
@@ -3429,7 +3416,7 @@
       <c r="AB38"/>
       <c r="AC38"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="39">
       <c r="A39" s="312"/>
       <c r="B39" s="70" t="s">
         <v>129</v>
@@ -3466,7 +3453,7 @@
       <c r="AB39" s="3"/>
       <c r="AC39" s="3"/>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="40">
       <c r="A40" s="312"/>
       <c r="B40" s="70" t="s">
         <v>129</v>
@@ -3486,7 +3473,7 @@
       <c r="K40" s="262"/>
       <c r="L40" s="29"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="41">
       <c r="A41" s="312"/>
       <c r="B41" s="281" t="s">
         <v>129</v>
@@ -3512,7 +3499,7 @@
       <c r="K41" s="262"/>
       <c r="L41" s="29"/>
     </row>
-    <row r="42" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" s="3" customFormat="true">
       <c r="A42" s="312"/>
       <c r="B42" s="70" t="s">
         <v>129</v>
@@ -3549,7 +3536,7 @@
       <c r="AB42"/>
       <c r="AC42"/>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="43">
       <c r="A43" s="312"/>
       <c r="B43" s="70" t="s">
         <v>129</v>
@@ -3586,7 +3573,7 @@
       <c r="AB43" s="3"/>
       <c r="AC43" s="3"/>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="44">
       <c r="A44" s="312"/>
       <c r="B44" s="70" t="s">
         <v>129</v>
@@ -3606,7 +3593,7 @@
       <c r="K44" s="262"/>
       <c r="L44" s="29"/>
     </row>
-    <row r="45" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" s="3" customFormat="true">
       <c r="A45" s="312"/>
       <c r="B45" s="72" t="s">
         <v>129</v>
@@ -3649,7 +3636,7 @@
       <c r="AB45"/>
       <c r="AC45"/>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="46">
       <c r="A46" s="312"/>
       <c r="B46" s="61" t="s">
         <v>100</v>
@@ -3694,7 +3681,7 @@
       <c r="AB46" s="3"/>
       <c r="AC46" s="3"/>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="47">
       <c r="A47" s="312"/>
       <c r="B47" s="61" t="s">
         <v>100</v>
@@ -3720,7 +3707,7 @@
       <c r="K47" s="262"/>
       <c r="L47" s="29"/>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="48">
       <c r="A48" s="312"/>
       <c r="B48" s="61" t="s">
         <v>100</v>
@@ -3746,7 +3733,7 @@
       <c r="K48" s="264"/>
       <c r="L48" s="29"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49">
       <c r="A49" s="312"/>
       <c r="B49" s="64" t="s">
         <v>100</v>
@@ -3772,7 +3759,7 @@
       <c r="K49" s="265"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50">
       <c r="A50" s="312"/>
       <c r="B50" s="67" t="s">
         <v>101</v>
@@ -3800,7 +3787,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51">
       <c r="A51" s="312"/>
       <c r="B51" s="70" t="s">
         <v>101</v>
@@ -3826,7 +3813,7 @@
       <c r="K51" s="264"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52">
       <c r="A52" s="312"/>
       <c r="B52" s="70" t="s">
         <v>101</v>
@@ -3852,7 +3839,7 @@
       <c r="K52" s="264"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53">
       <c r="A53" s="312"/>
       <c r="B53" s="70" t="s">
         <v>101</v>
@@ -3878,7 +3865,7 @@
       <c r="K53" s="264"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54">
       <c r="A54" s="312"/>
       <c r="B54" s="81" t="s">
         <v>127</v>
@@ -3898,7 +3885,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55">
       <c r="A55" s="312"/>
       <c r="B55" s="84" t="s">
         <v>128</v>
@@ -3918,7 +3905,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56">
       <c r="A56" s="312"/>
       <c r="B56" s="187" t="s">
         <v>84</v>
@@ -3945,7 +3932,7 @@
       <c r="K56" s="267"/>
       <c r="L56" s="4"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57">
       <c r="A57" s="312"/>
       <c r="B57" s="187" t="s">
         <v>129</v>
@@ -3965,7 +3952,7 @@
       <c r="K57" s="267"/>
       <c r="L57" s="4"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58">
       <c r="A58" s="312"/>
       <c r="B58" s="187" t="s">
         <v>129</v>
@@ -3985,7 +3972,7 @@
       <c r="K58" s="267"/>
       <c r="L58" s="4"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59">
       <c r="A59" s="312"/>
       <c r="B59" s="187" t="s">
         <v>129</v>
@@ -4005,7 +3992,7 @@
       <c r="K59" s="267"/>
       <c r="L59" s="4"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60">
       <c r="A60" s="312"/>
       <c r="B60" s="187" t="s">
         <v>129</v>
@@ -4034,7 +4021,7 @@
       <c r="K60" s="267"/>
       <c r="L60" s="4"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61">
       <c r="A61" s="312"/>
       <c r="B61" s="187" t="s">
         <v>129</v>
@@ -4054,7 +4041,7 @@
       <c r="K61" s="267"/>
       <c r="L61" s="4"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62">
       <c r="A62" s="312"/>
       <c r="B62" s="187" t="s">
         <v>129</v>
@@ -4074,7 +4061,7 @@
       <c r="K62" s="267"/>
       <c r="L62" s="4"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63">
       <c r="A63" s="312"/>
       <c r="B63" s="187" t="s">
         <v>129</v>
@@ -4094,7 +4081,7 @@
       <c r="K63" s="267"/>
       <c r="L63" s="4"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64">
       <c r="A64" s="312"/>
       <c r="B64" s="187" t="s">
         <v>129</v>
@@ -4123,7 +4110,7 @@
       <c r="K64" s="267"/>
       <c r="L64" s="4"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65">
       <c r="A65" s="312"/>
       <c r="B65" s="278" t="s">
         <v>100</v>
@@ -4152,7 +4139,7 @@
       <c r="K65" s="267"/>
       <c r="L65" s="4"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66">
       <c r="A66" s="312"/>
       <c r="B66" s="278" t="s">
         <v>100</v>
@@ -4181,7 +4168,7 @@
       <c r="K66" s="267"/>
       <c r="L66" s="4"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67">
       <c r="A67" s="312"/>
       <c r="B67" s="278" t="s">
         <v>100</v>
@@ -4210,7 +4197,7 @@
       <c r="K67" s="267"/>
       <c r="L67" s="4"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68">
       <c r="A68" s="312"/>
       <c r="B68" s="278" t="s">
         <v>100</v>
@@ -4239,7 +4226,7 @@
       <c r="K68" s="267"/>
       <c r="L68" s="4"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69">
       <c r="A69" s="312"/>
       <c r="B69" s="187" t="s">
         <v>101</v>
@@ -4268,7 +4255,7 @@
       <c r="K69" s="267"/>
       <c r="L69" s="4"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70">
       <c r="A70" s="312"/>
       <c r="B70" s="187" t="s">
         <v>101</v>
@@ -4297,7 +4284,7 @@
       <c r="K70" s="267"/>
       <c r="L70" s="4"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71">
       <c r="A71" s="312"/>
       <c r="B71" s="187" t="s">
         <v>101</v>
@@ -4326,7 +4313,7 @@
       <c r="K71" s="267"/>
       <c r="L71" s="4"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72">
       <c r="A72" s="312"/>
       <c r="B72" s="187" t="s">
         <v>101</v>
@@ -4355,7 +4342,7 @@
       <c r="K72" s="267"/>
       <c r="L72" s="4"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73">
       <c r="A73" s="312"/>
       <c r="B73" s="278" t="s">
         <v>127</v>
@@ -4373,7 +4360,7 @@
       <c r="K73" s="267"/>
       <c r="L73" s="4"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74">
       <c r="A74" s="312"/>
       <c r="B74" s="278" t="s">
         <v>128</v>
@@ -4391,7 +4378,7 @@
       <c r="K74" s="267"/>
       <c r="L74" s="4"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75">
       <c r="A75" s="312"/>
       <c r="B75" s="87" t="s">
         <v>84</v>
@@ -4429,7 +4416,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76">
       <c r="A76" s="312"/>
       <c r="B76" s="87" t="s">
         <v>129</v>
@@ -4466,7 +4453,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" ht="15" customHeight="true">
       <c r="A77" s="312"/>
       <c r="B77" s="90" t="s">
         <v>129</v>
@@ -4486,7 +4473,7 @@
       <c r="K77" s="262"/>
       <c r="L77" s="29"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78">
       <c r="A78" s="312"/>
       <c r="B78" s="90" t="s">
         <v>129</v>
@@ -4506,7 +4493,7 @@
       <c r="K78" s="262"/>
       <c r="L78" s="29"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79">
       <c r="A79" s="312"/>
       <c r="B79" s="90" t="s">
         <v>129</v>
@@ -4526,7 +4513,7 @@
       <c r="K79" s="262"/>
       <c r="L79" s="29"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="80">
       <c r="A80" s="312"/>
       <c r="B80" s="90" t="s">
         <v>129</v>
@@ -4546,7 +4533,7 @@
       <c r="K80" s="262"/>
       <c r="L80" s="29"/>
     </row>
-    <row r="81" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" ht="15" customHeight="true">
       <c r="A81" s="312"/>
       <c r="B81" s="90" t="s">
         <v>129</v>
@@ -4566,7 +4553,7 @@
       <c r="K81" s="262"/>
       <c r="L81" s="29"/>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="82">
       <c r="A82" s="312"/>
       <c r="B82" s="93" t="s">
         <v>129</v>
@@ -4601,7 +4588,7 @@
       <c r="K82" s="262"/>
       <c r="L82" s="29"/>
     </row>
-    <row r="83" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" s="3" customFormat="true">
       <c r="A83" s="312"/>
       <c r="B83" s="75" t="s">
         <v>100</v>
@@ -4655,7 +4642,7 @@
       <c r="AB83"/>
       <c r="AC83"/>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="84">
       <c r="A84" s="312"/>
       <c r="B84" s="77" t="s">
         <v>100</v>
@@ -4706,7 +4693,7 @@
       <c r="AB84" s="3"/>
       <c r="AC84" s="3"/>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="85">
       <c r="A85" s="312"/>
       <c r="B85" s="77" t="s">
         <v>100</v>
@@ -4741,7 +4728,7 @@
       <c r="K85" s="262"/>
       <c r="L85" s="29"/>
     </row>
-    <row r="86" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" s="3" customFormat="true">
       <c r="A86" s="312"/>
       <c r="B86" s="79" t="s">
         <v>100</v>
@@ -4792,7 +4779,7 @@
       <c r="AB86"/>
       <c r="AC86"/>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="87">
       <c r="A87" s="312"/>
       <c r="B87" s="90" t="s">
         <v>101</v>
@@ -4846,7 +4833,7 @@
       <c r="AB87" s="3"/>
       <c r="AC87" s="3"/>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="88">
       <c r="A88" s="312"/>
       <c r="B88" s="90" t="s">
         <v>101</v>
@@ -4881,7 +4868,7 @@
       <c r="K88" s="262"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" s="3" customFormat="true">
       <c r="A89" s="312"/>
       <c r="B89" s="90" t="s">
         <v>101</v>
@@ -4932,7 +4919,7 @@
       <c r="AB89"/>
       <c r="AC89"/>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="90">
       <c r="A90" s="312"/>
       <c r="B90" s="90" t="s">
         <v>101</v>
@@ -4984,7 +4971,7 @@
       <c r="AB90" s="3"/>
       <c r="AC90" s="3"/>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="91">
       <c r="A91" s="312"/>
       <c r="B91" s="75" t="s">
         <v>127</v>
@@ -5004,7 +4991,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="92">
       <c r="A92" s="312"/>
       <c r="B92" s="79" t="s">
         <v>128</v>
@@ -5024,7 +5011,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="93" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" ht="15.75" customHeight="true">
       <c r="A93" s="312"/>
       <c r="B93" s="137" t="s">
         <v>84</v>
@@ -5059,7 +5046,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="94" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" ht="15" customHeight="true">
       <c r="A94" s="312"/>
       <c r="B94" s="144" t="s">
         <v>129</v>
@@ -5079,7 +5066,7 @@
       <c r="K94" s="252"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" ht="15" customHeight="true">
       <c r="A95" s="312"/>
       <c r="B95" s="147" t="s">
         <v>129</v>
@@ -5099,7 +5086,7 @@
       <c r="K95" s="252"/>
       <c r="L95" s="3"/>
     </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="96">
       <c r="A96" s="312"/>
       <c r="B96" s="147" t="s">
         <v>129</v>
@@ -5119,7 +5106,7 @@
       <c r="K96" s="252"/>
       <c r="L96" s="3"/>
     </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="97">
       <c r="A97" s="312"/>
       <c r="B97" s="147" t="s">
         <v>129</v>
@@ -5139,7 +5126,7 @@
       <c r="K97" s="252"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="98" s="3" customFormat="true">
       <c r="A98" s="312"/>
       <c r="B98" s="147" t="s">
         <v>129</v>
@@ -5191,7 +5178,7 @@
       <c r="AB98"/>
       <c r="AC98"/>
     </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="99">
       <c r="A99" s="312"/>
       <c r="B99" s="147" t="s">
         <v>129</v>
@@ -5240,7 +5227,7 @@
       <c r="AB99" s="3"/>
       <c r="AC99" s="3"/>
     </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="100">
       <c r="A100" s="312"/>
       <c r="B100" s="150" t="s">
         <v>129</v>
@@ -5275,7 +5262,7 @@
       <c r="K100" s="252"/>
       <c r="L100" s="4"/>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="101">
       <c r="A101" s="312"/>
       <c r="B101" s="137" t="s">
         <v>100</v>
@@ -5310,7 +5297,7 @@
       <c r="K101" s="252"/>
       <c r="L101" s="4"/>
     </row>
-    <row r="102" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="102" s="3" customFormat="true">
       <c r="A102" s="312"/>
       <c r="B102" s="139" t="s">
         <v>100</v>
@@ -5359,7 +5346,7 @@
       <c r="AB102"/>
       <c r="AC102"/>
     </row>
-    <row r="103" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="103" s="3" customFormat="true">
       <c r="A103" s="312"/>
       <c r="B103" s="139" t="s">
         <v>100</v>
@@ -5394,7 +5381,7 @@
       <c r="K103" s="252"/>
       <c r="L103" s="28"/>
     </row>
-    <row r="104" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="104" s="3" customFormat="true">
       <c r="A104" s="312"/>
       <c r="B104" s="141" t="s">
         <v>100</v>
@@ -5426,7 +5413,7 @@
       <c r="K104" s="252"/>
       <c r="L104" s="28"/>
     </row>
-    <row r="105" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="105" s="3" customFormat="true">
       <c r="A105" s="312"/>
       <c r="B105" s="147" t="s">
         <v>101</v>
@@ -5461,7 +5448,7 @@
       <c r="K105" s="252"/>
       <c r="L105" s="28"/>
     </row>
-    <row r="106" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="106" s="3" customFormat="true">
       <c r="A106" s="312"/>
       <c r="B106" s="147" t="s">
         <v>101</v>
@@ -5481,7 +5468,7 @@
       <c r="K106" s="252"/>
       <c r="L106" s="28"/>
     </row>
-    <row r="107" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="107" s="3" customFormat="true">
       <c r="A107" s="312"/>
       <c r="B107" s="147" t="s">
         <v>101</v>
@@ -5501,7 +5488,7 @@
       <c r="K107" s="252"/>
       <c r="L107" s="4"/>
     </row>
-    <row r="108" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="108" s="3" customFormat="true">
       <c r="A108" s="312"/>
       <c r="B108" s="147" t="s">
         <v>101</v>
@@ -5521,7 +5508,7 @@
       <c r="K108" s="252"/>
       <c r="L108" s="4"/>
     </row>
-    <row r="109" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="109" s="3" customFormat="true">
       <c r="A109" s="312"/>
       <c r="B109" s="137" t="s">
         <v>127</v>
@@ -5539,7 +5526,7 @@
       <c r="K109" s="271"/>
       <c r="L109" s="4"/>
     </row>
-    <row r="110" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="110" s="3" customFormat="true">
       <c r="A110" s="312"/>
       <c r="B110" s="141" t="s">
         <v>128</v>
@@ -5557,7 +5544,7 @@
       <c r="K110" s="272"/>
       <c r="L110" s="4"/>
     </row>
-    <row r="111" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="111" s="3" customFormat="true">
       <c r="A111" s="312"/>
       <c r="B111" s="162" t="s">
         <v>84</v>
@@ -5592,7 +5579,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="112" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="112" s="3" customFormat="true">
       <c r="A112" s="312"/>
       <c r="B112" s="153" t="s">
         <v>129</v>
@@ -5612,7 +5599,7 @@
       <c r="K112" s="252"/>
       <c r="L112" s="4"/>
     </row>
-    <row r="113" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="113" s="3" customFormat="true">
       <c r="A113" s="312"/>
       <c r="B113" s="156" t="s">
         <v>129</v>
@@ -5632,7 +5619,7 @@
       <c r="K113" s="252"/>
       <c r="L113" s="4"/>
     </row>
-    <row r="114" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="114" s="3" customFormat="true">
       <c r="A114" s="312"/>
       <c r="B114" s="156" t="s">
         <v>129</v>
@@ -5652,7 +5639,7 @@
       <c r="K114" s="252"/>
       <c r="L114" s="4"/>
     </row>
-    <row r="115" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="115" s="3" customFormat="true">
       <c r="A115" s="312"/>
       <c r="B115" s="156" t="s">
         <v>129</v>
@@ -5672,7 +5659,7 @@
       <c r="K115" s="252"/>
       <c r="L115" s="4"/>
     </row>
-    <row r="116" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="116" s="3" customFormat="true">
       <c r="A116" s="312"/>
       <c r="B116" s="156" t="s">
         <v>129</v>
@@ -5707,7 +5694,7 @@
       <c r="K116" s="252"/>
       <c r="L116" s="4"/>
     </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="117">
       <c r="A117" s="312"/>
       <c r="B117" s="156" t="s">
         <v>129</v>
@@ -5744,7 +5731,7 @@
       <c r="AB117" s="3"/>
       <c r="AC117" s="3"/>
     </row>
-    <row r="118" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="118">
       <c r="A118" s="312"/>
       <c r="B118" s="159" t="s">
         <v>129</v>
@@ -5779,7 +5766,7 @@
       <c r="K118" s="252"/>
       <c r="L118" s="4"/>
     </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="119">
       <c r="A119" s="312"/>
       <c r="B119" s="162" t="s">
         <v>100</v>
@@ -5814,7 +5801,7 @@
       <c r="K119" s="273"/>
       <c r="L119" s="4"/>
     </row>
-    <row r="120" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="120" s="3" customFormat="true">
       <c r="A120" s="312"/>
       <c r="B120" s="165" t="s">
         <v>100</v>
@@ -5851,7 +5838,7 @@
       <c r="AB120"/>
       <c r="AC120"/>
     </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="121">
       <c r="A121" s="312"/>
       <c r="B121" s="165" t="s">
         <v>100</v>
@@ -5903,7 +5890,7 @@
       <c r="AB121" s="3"/>
       <c r="AC121" s="3"/>
     </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="122">
       <c r="A122" s="312"/>
       <c r="B122" s="167" t="s">
         <v>100</v>
@@ -5923,7 +5910,7 @@
       <c r="K122" s="274"/>
       <c r="L122" s="4"/>
     </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="123">
       <c r="A123" s="312"/>
       <c r="B123" s="156" t="s">
         <v>101</v>
@@ -5958,7 +5945,7 @@
       <c r="K123" s="252"/>
       <c r="L123" s="4"/>
     </row>
-    <row r="124" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="124">
       <c r="A124" s="312"/>
       <c r="B124" s="156" t="s">
         <v>101</v>
@@ -5978,7 +5965,7 @@
       <c r="K124" s="252"/>
       <c r="L124" s="4"/>
     </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="125">
       <c r="A125" s="312"/>
       <c r="B125" s="156" t="s">
         <v>101</v>
@@ -5998,7 +5985,7 @@
       <c r="K125" s="252"/>
       <c r="L125" s="4"/>
     </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="126">
       <c r="A126" s="312"/>
       <c r="B126" s="156" t="s">
         <v>101</v>
@@ -6018,7 +6005,7 @@
       <c r="K126" s="252"/>
       <c r="L126" s="4"/>
     </row>
-    <row r="127" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" ht="15" customHeight="true">
       <c r="A127" s="312"/>
       <c r="B127" s="162" t="s">
         <v>127</v>
@@ -6036,7 +6023,7 @@
       <c r="K127" s="263"/>
       <c r="L127" s="4"/>
     </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="128">
       <c r="A128" s="312"/>
       <c r="B128" s="167" t="s">
         <v>128</v>
@@ -6054,7 +6041,7 @@
       <c r="K128" s="265"/>
       <c r="L128" s="4"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="129">
       <c r="A129" s="312"/>
       <c r="B129" s="173" t="s">
         <v>84</v>
@@ -6089,7 +6076,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="130">
       <c r="A130" s="312"/>
       <c r="B130" s="184" t="s">
         <v>129</v>
@@ -6109,7 +6096,7 @@
       <c r="K130" s="252"/>
       <c r="L130" s="4"/>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="131">
       <c r="A131" s="312"/>
       <c r="B131" s="187" t="s">
         <v>129</v>
@@ -6129,7 +6116,7 @@
       <c r="K131" s="252"/>
       <c r="L131" s="4"/>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="132">
       <c r="A132" s="312"/>
       <c r="B132" s="187" t="s">
         <v>129</v>
@@ -6149,7 +6136,7 @@
       <c r="K132" s="252"/>
       <c r="L132" s="4"/>
     </row>
-    <row r="133" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" ht="15" customHeight="true">
       <c r="A133" s="312"/>
       <c r="B133" s="187" t="s">
         <v>129</v>
@@ -6169,7 +6156,7 @@
       <c r="K133" s="252"/>
       <c r="L133" s="4"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="134">
       <c r="A134" s="312"/>
       <c r="B134" s="187" t="s">
         <v>129</v>
@@ -6204,7 +6191,7 @@
       <c r="K134" s="252"/>
       <c r="L134" s="4"/>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="135">
       <c r="A135" s="312"/>
       <c r="B135" s="187" t="s">
         <v>129</v>
@@ -6224,7 +6211,7 @@
       <c r="K135" s="252"/>
       <c r="L135" s="30"/>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="136">
       <c r="A136" s="312"/>
       <c r="B136" s="190" t="s">
         <v>129</v>
@@ -6259,7 +6246,7 @@
       <c r="K136" s="252"/>
       <c r="L136" s="4"/>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="137">
       <c r="A137" s="312"/>
       <c r="B137" s="173" t="s">
         <v>100</v>
@@ -6294,7 +6281,7 @@
       <c r="K137" s="273"/>
       <c r="L137" s="4"/>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="138">
       <c r="A138" s="312"/>
       <c r="B138" s="176" t="s">
         <v>100</v>
@@ -6314,7 +6301,7 @@
       <c r="K138" s="252"/>
       <c r="L138" s="4"/>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="139">
       <c r="A139" s="312"/>
       <c r="B139" s="176" t="s">
         <v>100</v>
@@ -6349,7 +6336,7 @@
       <c r="K139" s="252"/>
       <c r="L139" s="4"/>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="140">
       <c r="A140" s="312"/>
       <c r="B140" s="178" t="s">
         <v>100</v>
@@ -6369,7 +6356,7 @@
       <c r="K140" s="274"/>
       <c r="L140" s="4"/>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="141">
       <c r="A141" s="312"/>
       <c r="B141" s="187" t="s">
         <v>101</v>
@@ -6404,7 +6391,7 @@
       <c r="K141" s="252"/>
       <c r="L141" s="215"/>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="142">
       <c r="A142" s="312"/>
       <c r="B142" s="187" t="s">
         <v>101</v>
@@ -6424,7 +6411,7 @@
       <c r="K142" s="252"/>
       <c r="L142" s="215"/>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="143">
       <c r="A143" s="312"/>
       <c r="B143" s="187" t="s">
         <v>101</v>
@@ -6444,7 +6431,7 @@
       <c r="K143" s="252"/>
       <c r="L143" s="4"/>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="144">
       <c r="A144" s="312"/>
       <c r="B144" s="187" t="s">
         <v>101</v>
@@ -6464,7 +6451,7 @@
       <c r="K144" s="252"/>
       <c r="L144" s="40"/>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="145">
       <c r="A145" s="312"/>
       <c r="B145" s="173" t="s">
         <v>127</v>
@@ -6482,7 +6469,7 @@
       <c r="K145" s="263"/>
       <c r="L145" s="4"/>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="146">
       <c r="A146" s="313"/>
       <c r="B146" s="178" t="s">
         <v>128</v>
@@ -6500,7 +6487,7 @@
       <c r="K146" s="265"/>
       <c r="L146" s="40"/>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="147">
       <c r="A147" s="314" t="s">
         <v>142</v>
       </c>
@@ -6520,7 +6507,7 @@
       <c r="K147" s="275"/>
       <c r="L147" s="4"/>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="148">
       <c r="A148" s="315"/>
       <c r="B148" s="243" t="s">
         <v>12</v>
@@ -6537,7 +6524,7 @@
       <c r="J148" s="231"/>
       <c r="L148" s="4"/>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="149">
       <c r="A149" s="315"/>
       <c r="B149" s="243" t="s">
         <v>12</v>
@@ -6553,7 +6540,7 @@
       <c r="I149" s="230"/>
       <c r="J149" s="231"/>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="150">
       <c r="A150" s="315"/>
       <c r="B150" s="236" t="s">
         <v>134</v>
@@ -6586,7 +6573,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="151">
       <c r="A151" s="315"/>
       <c r="B151" s="243" t="s">
         <v>15</v>
@@ -6602,7 +6589,7 @@
       <c r="I151" s="230"/>
       <c r="J151" s="231"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="152">
       <c r="A152" s="315"/>
       <c r="B152" s="243" t="s">
         <v>16</v>
@@ -6618,7 +6605,7 @@
       <c r="I152" s="230"/>
       <c r="J152" s="231"/>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="153">
       <c r="A153" s="316"/>
       <c r="B153" s="244" t="s">
         <v>17</v>
@@ -6635,7 +6622,7 @@
       <c r="J153" s="247"/>
       <c r="K153" s="277"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="154">
       <c r="A154" s="317" t="s">
         <v>143</v>
       </c>
@@ -6646,7 +6633,7 @@
       <c r="D154" s="3"/>
       <c r="E154" s="3"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="155">
       <c r="A155" s="317"/>
       <c r="B155" s="3" t="s">
         <v>21</v>
@@ -6655,7 +6642,7 @@
       <c r="D155" s="3"/>
       <c r="E155" s="3"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="156">
       <c r="A156" s="317"/>
       <c r="B156" s="3" t="s">
         <v>22</v>
@@ -6664,7 +6651,7 @@
       <c r="D156" s="3"/>
       <c r="E156" s="3"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="157">
       <c r="A157" s="317"/>
       <c r="B157" s="3" t="s">
         <v>23</v>
@@ -6673,7 +6660,7 @@
       <c r="D157" s="3"/>
       <c r="E157" s="3"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="158">
       <c r="A158" s="317"/>
       <c r="B158" s="3" t="s">
         <v>24</v>
@@ -6682,7 +6669,7 @@
       <c r="D158" s="3"/>
       <c r="E158" s="3"/>
     </row>
-    <row r="159" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" ht="14.25" customHeight="true">
       <c r="A159" s="317"/>
       <c r="B159" s="3" t="s">
         <v>52</v>
@@ -6691,7 +6678,7 @@
       <c r="D159" s="3"/>
       <c r="E159" s="3"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="160">
       <c r="A160" s="317"/>
       <c r="B160" s="10" t="s">
         <v>47</v>
@@ -6702,7 +6689,7 @@
       <c r="D160" s="9"/>
       <c r="E160" s="9"/>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161">
       <c r="A161" s="317"/>
       <c r="B161" s="10" t="s">
         <v>48</v>
@@ -6711,7 +6698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162">
       <c r="A162" s="317"/>
       <c r="B162" s="10" t="s">
         <v>47</v>
@@ -6720,7 +6707,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163">
       <c r="A163" s="317"/>
       <c r="B163" s="10" t="s">
         <v>48</v>
@@ -6731,7 +6718,7 @@
       <c r="D163" s="9"/>
       <c r="E163" s="9"/>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="164">
       <c r="A164" s="317"/>
       <c r="B164" t="s">
         <v>50</v>
@@ -6742,7 +6729,7 @@
       <c r="D164" s="9"/>
       <c r="E164" s="9"/>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="165">
       <c r="A165" s="317"/>
       <c r="B165" t="s">
         <v>51</v>
@@ -6753,61 +6740,61 @@
       <c r="D165" s="9"/>
       <c r="E165" s="9"/>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166">
       <c r="D166" s="9"/>
       <c r="E166" s="9"/>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167">
       <c r="D167" s="9"/>
       <c r="E167" s="9"/>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168">
       <c r="D168" s="9"/>
       <c r="E168" s="9"/>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169">
       <c r="B169" s="11"/>
       <c r="C169" s="3"/>
       <c r="D169" s="3"/>
       <c r="E169" s="9"/>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170">
       <c r="B170" s="11"/>
       <c r="C170" s="3"/>
       <c r="D170" s="3"/>
       <c r="E170" s="9"/>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171">
       <c r="B171" s="11"/>
       <c r="C171" s="3"/>
       <c r="D171" s="3"/>
       <c r="E171" s="9"/>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172">
       <c r="B172" s="11"/>
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
       <c r="E172" s="9"/>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173">
       <c r="B173" s="11"/>
       <c r="C173" s="3"/>
       <c r="D173" s="3"/>
       <c r="E173" s="9"/>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174">
       <c r="B174" s="11"/>
       <c r="C174" s="3"/>
       <c r="D174" s="3"/>
       <c r="E174" s="3"/>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175">
       <c r="B175" s="11"/>
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
       <c r="E175" s="3"/>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176">
       <c r="B176" s="11"/>
       <c r="C176" s="3"/>
       <c r="D176" s="3"/>
@@ -6831,21 +6818,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="14.26953125" customWidth="1"/>
-    <col min="3" max="4" width="11.453125" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" customWidth="true"/>
+    <col min="3" max="4" width="11.453125" customWidth="true"/>
+    <col min="6" max="6" width="10.54296875" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="C4" t="s">
         <v>150</v>
       </c>
@@ -6862,7 +6849,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5">
       <c r="B5" t="s">
         <v>148</v>
       </c>
@@ -6882,7 +6869,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="6">
       <c r="B6" t="s">
         <v>149</v>
       </c>
@@ -6908,21 +6895,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="5" width="10.54296875" customWidth="1"/>
-    <col min="6" max="8" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="true"/>
+    <col min="3" max="5" width="10.54296875" customWidth="true"/>
+    <col min="6" max="8" width="13.7265625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="B1" s="13" t="s">
         <v>78</v>
       </c>
@@ -6933,7 +6920,7 @@
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="C2" t="s">
         <v>150</v>
       </c>
@@ -6950,7 +6937,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -6974,7 +6961,7 @@
       </c>
       <c r="H3" s="15"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -6998,7 +6985,7 @@
       </c>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -7022,7 +7009,7 @@
       </c>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -7046,7 +7033,7 @@
       </c>
       <c r="H6" s="15"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -7070,7 +7057,7 @@
       </c>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -7094,7 +7081,7 @@
       </c>
       <c r="H8" s="15"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -7118,7 +7105,7 @@
       </c>
       <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10">
       <c r="C10" s="31">
         <f>SUM(C3:C9)</f>
         <v>51.389299484955423</v>
@@ -7141,12 +7128,12 @@
       </c>
       <c r="H10" s="31"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12">
       <c r="B12" s="13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13">
       <c r="C13" t="str">
         <f>C2</f>
         <v>AquaFSm</v>
@@ -7168,7 +7155,7 @@
         <v>AquaLL</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -7197,7 +7184,7 @@
       </c>
       <c r="H14" s="32"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15">
       <c r="A15" t="s">
         <v>85</v>
       </c>
@@ -7226,7 +7213,7 @@
       </c>
       <c r="H15" s="32"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -7255,7 +7242,7 @@
       </c>
       <c r="H16" s="32"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -7284,7 +7271,7 @@
       </c>
       <c r="H17" s="32"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -7313,7 +7300,7 @@
       </c>
       <c r="H18" s="32"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19">
       <c r="A19" t="s">
         <v>87</v>
       </c>
@@ -7342,7 +7329,7 @@
       </c>
       <c r="H19" s="32"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -7377,20 +7364,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="17.54296875" customWidth="1"/>
-    <col min="3" max="8" width="13.26953125" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" customWidth="true"/>
+    <col min="3" max="8" width="13.26953125" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="C1" s="23" t="s">
         <v>72</v>
       </c>
@@ -7398,7 +7385,7 @@
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="C2" t="s">
         <v>150</v>
       </c>
@@ -7412,7 +7399,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3">
       <c r="B3" t="s">
         <v>73</v>
       </c>
@@ -7432,7 +7419,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7">
       <c r="C7" s="23" t="s">
         <v>165</v>
       </c>
@@ -7440,7 +7427,7 @@
       <c r="E7" s="23"/>
       <c r="F7" s="23"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8">
       <c r="C8" t="s">
         <v>150</v>
       </c>
@@ -7451,7 +7438,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9">
       <c r="C9" t="s">
         <v>8</v>
       </c>
@@ -7462,7 +7449,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10">
       <c r="B10" t="s">
         <v>61</v>
       </c>
@@ -7470,7 +7457,7 @@
         <v>0.17072752641725361</v>
       </c>
       <c r="D10" s="18">
-        <v>2.7781796293062627E-2</v>
+        <v>0.027781796293067068</v>
       </c>
       <c r="E10" s="18">
         <v>0.17393061946984731</v>
@@ -7480,15 +7467,15 @@
       <c r="H10" s="20"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11">
       <c r="B11" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="18">
-        <v>0.34537448398886794</v>
+        <v>0.34537448398886766</v>
       </c>
       <c r="D11" s="18">
-        <v>0.27965573781579067</v>
+        <v>0.27965573781578135</v>
       </c>
       <c r="E11" s="18">
         <v>0.49597818331189858</v>
@@ -7498,25 +7485,25 @@
       <c r="H11" s="20"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12">
       <c r="B12" t="s">
         <v>63</v>
       </c>
       <c r="C12" s="18">
-        <v>-4.2695223915633629E-2</v>
+        <v>-0.042695223915634073</v>
       </c>
       <c r="D12" s="18">
-        <v>7.3137310251506604E-2</v>
+        <v>0.073137310251512822</v>
       </c>
       <c r="E12" s="18">
-        <v>3.1023585864751957E-2</v>
+        <v>0.031023585864751957</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="20"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13">
       <c r="B13" t="s">
         <v>64</v>
       </c>
@@ -7534,12 +7521,12 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14">
       <c r="B14" t="s">
         <v>59</v>
       </c>
       <c r="C14" s="14">
-        <v>1.8092917424992319</v>
+        <v>1.8092917424992301</v>
       </c>
       <c r="D14" s="14">
         <v>1.716711144133658</v>
@@ -7554,7 +7541,7 @@
       <c r="H14" s="20"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15">
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
       <c r="F15" s="3"/>
@@ -7562,7 +7549,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="19">
       <c r="C19" s="23" t="s">
         <v>150</v>
       </c>
@@ -7574,7 +7561,7 @@
       </c>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="20">
       <c r="C20" t="s">
         <v>150</v>
       </c>
@@ -7585,7 +7572,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" ht="14.25" customHeight="true">
       <c r="C21" t="s">
         <v>9</v>
       </c>
@@ -7596,71 +7583,71 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" ht="14.25" customHeight="true">
       <c r="B22" t="s">
         <v>61</v>
       </c>
       <c r="C22" s="19">
-        <v>8.7745223232686131E-2</v>
+        <v>0.087745223232685826</v>
       </c>
       <c r="D22" s="19">
-        <v>0.10309217333282318</v>
+        <v>0.10309217333282217</v>
       </c>
       <c r="E22" s="19">
         <v>0.11976329294262</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" ht="14.25" customHeight="true">
       <c r="B23" t="s">
         <v>62</v>
       </c>
       <c r="C23" s="19">
-        <v>8.8287564119833975E-2</v>
+        <v>0.0882875641198336</v>
       </c>
       <c r="D23" s="19">
-        <v>9.7593564718067197E-2</v>
+        <v>0.097593564718066045</v>
       </c>
       <c r="E23" s="19">
         <v>0.1785079900871287</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" ht="14.25" customHeight="true">
       <c r="B24" t="s">
         <v>63</v>
       </c>
       <c r="C24" s="19">
-        <v>4.1310825018677791E-2</v>
+        <v>0.04131082501867761</v>
       </c>
       <c r="D24" s="19">
-        <v>4.4894911686997351E-2</v>
+        <v>0.044894911686997593</v>
       </c>
       <c r="E24" s="19">
         <v>0.15453056276912325</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="25">
       <c r="B25" t="s">
         <v>64</v>
       </c>
       <c r="C25" s="19">
-        <v>7.226500839942547E-2</v>
+        <v>0.072265008399425484</v>
       </c>
       <c r="D25" s="19">
-        <v>6.1518913298974097E-2</v>
+        <v>0.061518913298975457</v>
       </c>
       <c r="E25" s="19">
         <v>0.21660166504423975</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="26">
       <c r="B26" t="s">
         <v>59</v>
       </c>
       <c r="C26">
-        <v>0.20201988981837676</v>
+        <v>0.20201988981837624</v>
       </c>
       <c r="D26">
-        <v>0.1703713981690903</v>
+        <v>0.17037139816909169</v>
       </c>
       <c r="E26">
         <v>0.39848951125761112</v>
@@ -7669,7 +7656,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="30">
       <c r="C30" s="23" t="s">
         <v>161</v>
       </c>
@@ -7677,7 +7664,7 @@
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="31">
       <c r="C31" t="s">
         <v>150</v>
       </c>
@@ -7688,7 +7675,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="32">
       <c r="B32" t="s">
         <v>168</v>
       </c>
@@ -7696,13 +7683,13 @@
         <v>0.11411485697008658</v>
       </c>
       <c r="D32" s="32">
-        <v>8.9996141320724879E-2</v>
+        <v>0.089996141320724879</v>
       </c>
       <c r="E32" s="32">
         <v>0.54471593702583854</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33">
       <c r="B33" t="s">
         <v>162</v>
       </c>
@@ -7710,13 +7697,13 @@
         <v>0.15026443869660544</v>
       </c>
       <c r="D33" s="32">
-        <v>8.2452484663229297E-2</v>
+        <v>0.082452484663229297</v>
       </c>
       <c r="E33" s="32">
         <v>0.27530932263038205</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="36">
       <c r="C36" s="13" t="s">
         <v>163</v>
       </c>
@@ -7724,7 +7711,7 @@
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
     </row>
-    <row r="68" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="68">
       <c r="H68" s="305" t="e">
         <f>Fish!E22:E25</f>
         <v>#VALUE!</v>
@@ -7736,43 +7723,43 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16" style="5" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="10" style="5" customWidth="1"/>
-    <col min="10" max="10" width="7.81640625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="11.54296875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="6.81640625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="10.7265625" style="5" customWidth="1"/>
-    <col min="14" max="14" width="10" style="5" customWidth="1"/>
-    <col min="15" max="15" width="7.81640625" style="5" customWidth="1"/>
-    <col min="16" max="16" width="12.54296875" style="5" customWidth="1"/>
-    <col min="17" max="17" width="9.1796875" style="5" customWidth="1"/>
-    <col min="18" max="18" width="11" style="5" customWidth="1"/>
-    <col min="19" max="19" width="9.453125" style="5" customWidth="1"/>
-    <col min="20" max="20" width="10" style="5" customWidth="1"/>
-    <col min="21" max="21" width="12.54296875" style="5" customWidth="1"/>
-    <col min="22" max="22" width="8.7265625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="20" style="5" customWidth="true"/>
+    <col min="2" max="2" width="10" style="5" customWidth="true"/>
+    <col min="3" max="3" width="16" style="5" customWidth="true"/>
+    <col min="4" max="4" width="15.26953125" style="5" customWidth="true"/>
+    <col min="5" max="5" width="14.54296875" style="5" customWidth="true"/>
+    <col min="6" max="6" width="14.81640625" style="5" customWidth="true"/>
+    <col min="7" max="7" width="14.26953125" style="5" customWidth="true"/>
+    <col min="8" max="8" width="9.1796875" style="5" customWidth="true"/>
+    <col min="9" max="9" width="10" style="5" customWidth="true"/>
+    <col min="10" max="10" width="7.81640625" style="5" customWidth="true"/>
+    <col min="11" max="11" width="11.54296875" style="5" customWidth="true"/>
+    <col min="12" max="12" width="6.81640625" style="5" customWidth="true"/>
+    <col min="13" max="13" width="10.7265625" style="5" customWidth="true"/>
+    <col min="14" max="14" width="10" style="5" customWidth="true"/>
+    <col min="15" max="15" width="7.81640625" style="5" customWidth="true"/>
+    <col min="16" max="16" width="12.54296875" style="5" customWidth="true"/>
+    <col min="17" max="17" width="9.1796875" style="5" customWidth="true"/>
+    <col min="18" max="18" width="11" style="5" customWidth="true"/>
+    <col min="19" max="19" width="9.453125" style="5" customWidth="true"/>
+    <col min="20" max="20" width="10" style="5" customWidth="true"/>
+    <col min="21" max="21" width="12.54296875" style="5" customWidth="true"/>
+    <col min="22" max="22" width="8.7265625" style="5" customWidth="true"/>
     <col min="23" max="25" width="9.1796875" style="5"/>
-    <col min="26" max="26" width="15.26953125" style="5" customWidth="1"/>
+    <col min="26" max="26" width="15.26953125" style="5" customWidth="true"/>
     <col min="27" max="16384" width="9.1796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="B1" s="23" t="s">
         <v>72</v>
       </c>
@@ -7781,7 +7768,7 @@
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="C2" t="s">
         <v>150</v>
       </c>
@@ -7801,7 +7788,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="3">
       <c r="B3" t="s">
         <v>74</v>
       </c>
@@ -7822,7 +7809,7 @@
       </c>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="B4" t="s">
         <v>160</v>
       </c>
@@ -7843,7 +7830,7 @@
       </c>
       <c r="H4"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="7">
       <c r="B7" s="23" t="s">
         <v>71</v>
       </c>
@@ -7852,7 +7839,7 @@
       <c r="E7" s="23"/>
       <c r="F7" s="23"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="8">
       <c r="B8"/>
       <c r="C8" t="s">
         <v>152</v>
@@ -7874,7 +7861,7 @@
       </c>
       <c r="K8" s="26"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="9">
       <c r="B9"/>
       <c r="C9" t="s">
         <v>8</v>
@@ -7896,7 +7883,7 @@
       </c>
       <c r="K9" s="26"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="10">
       <c r="B10" t="s">
         <v>61</v>
       </c>
@@ -7916,7 +7903,7 @@
       <c r="L10"/>
       <c r="M10" s="16"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="11">
       <c r="B11" t="s">
         <v>62</v>
       </c>
@@ -7936,7 +7923,7 @@
       <c r="L11"/>
       <c r="M11" s="16"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="12">
       <c r="B12" t="s">
         <v>63</v>
       </c>
@@ -7956,7 +7943,7 @@
       <c r="L12"/>
       <c r="M12" s="16"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="13">
       <c r="B13" t="s">
         <v>64</v>
       </c>
@@ -7976,7 +7963,7 @@
       <c r="L13"/>
       <c r="M13" s="16"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="14">
       <c r="B14" t="s">
         <v>59</v>
       </c>
@@ -7995,10 +7982,10 @@
       <c r="K14" s="14"/>
       <c r="L14"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="15">
       <c r="K15" s="26"/>
     </row>
-    <row r="19" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" ht="18.75" customHeight="true">
       <c r="B19"/>
       <c r="C19" s="23" t="s">
         <v>161</v>
@@ -8007,7 +7994,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" ht="18.75" customHeight="true">
       <c r="B20"/>
       <c r="C20" t="s">
         <v>150</v>
@@ -8025,7 +8012,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" ht="18.75" customHeight="true">
       <c r="B21" t="s">
         <v>175</v>
       </c>
@@ -8037,7 +8024,7 @@
       </c>
       <c r="G21"/>
     </row>
-    <row r="22" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" ht="18.75" customHeight="true">
       <c r="B22" t="s">
         <v>162</v>
       </c>
@@ -8049,30 +8036,30 @@
       </c>
       <c r="G22"/>
     </row>
-    <row r="23" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" ht="18.75" customHeight="true"/>
+    <row r="24" ht="18.75" customHeight="true"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="3" max="3" width="19.26953125" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="true"/>
+    <col min="2" max="2" width="15.81640625" customWidth="true"/>
+    <col min="3" max="3" width="19.26953125" customWidth="true"/>
+    <col min="4" max="4" width="16.7265625" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2">
       <c r="C2" t="s">
         <v>150</v>
       </c>
@@ -8092,7 +8079,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3">
       <c r="B3" t="s">
         <v>110</v>
       </c>
@@ -8115,7 +8102,7 @@
         <v>18.116273880004883</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="B4" t="s">
         <v>69</v>
       </c>
@@ -8135,7 +8122,7 @@
         <v>19.261402130126953</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5">
       <c r="B5" t="s">
         <v>111</v>
       </c>
@@ -8158,7 +8145,7 @@
         <v>93.977943420410156</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" ht="29">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -8190,7 +8177,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9">
       <c r="C9" t="s">
         <v>68</v>
       </c>
@@ -8219,7 +8206,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -8254,7 +8241,7 @@
         <v>6.6375721112827385E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11">
       <c r="B11" t="s">
         <v>59</v>
       </c>
@@ -8286,7 +8273,7 @@
         <v>6.0673880015572905E-8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -8312,7 +8299,7 @@
       <c r="J12" s="14"/>
       <c r="K12" s="17"/>
     </row>
-    <row r="20" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" ht="29">
       <c r="C20" s="7" t="s">
         <v>172</v>
       </c>
@@ -8320,7 +8307,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="21">
       <c r="B21" t="s">
         <v>67</v>
       </c>
@@ -8331,7 +8318,7 @@
         <v>0.38204139885705091</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="22">
       <c r="B22" t="s">
         <v>69</v>
       </c>
@@ -8342,7 +8329,7 @@
         <v>0.38126708309476026</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="23">
       <c r="B23" t="s">
         <v>70</v>
       </c>
@@ -8353,7 +8340,7 @@
         <v>0.55383863325815852</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" ht="43.5">
       <c r="C25" s="8" t="s">
         <v>112</v>
       </c>
@@ -8361,7 +8348,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="26">
       <c r="B26" t="s">
         <v>67</v>
       </c>
@@ -8374,7 +8361,7 @@
         <v>0.14828300141565628</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="27">
       <c r="B27" t="s">
         <v>69</v>
       </c>
@@ -8387,7 +8374,7 @@
         <v>0.1363825833664721</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="28">
       <c r="B28" t="s">
         <v>70</v>
       </c>
@@ -8406,16 +8393,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="C4" t="s">
         <v>152</v>
       </c>
@@ -8435,7 +8422,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="5">
       <c r="B5" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
Fixed RAR for paper
</commit_message>
<xml_diff>
--- a/GAMS/AQ_LEWIE_InputSheet.xlsx
+++ b/GAMS/AQ_LEWIE_InputSheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="21150" windowHeight="6260" tabRatio="736" activeTab="5"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="176">
   <si>
     <t>Variable</t>
   </si>
@@ -2423,10 +2423,10 @@
   <dimension ref="A1:AC176"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J86" sqref="J86"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3654,7 +3654,7 @@
       </c>
       <c r="G46" s="114">
         <f>Fish!D10</f>
-        <v>2.7781796293062627E-2</v>
+        <v>2.7781796293067068E-2</v>
       </c>
       <c r="H46" s="41"/>
       <c r="I46" s="41"/>
@@ -3695,11 +3695,11 @@
       </c>
       <c r="F47" s="109">
         <f>Fish!C11</f>
-        <v>0.34537448398886794</v>
+        <v>0.34537448398886766</v>
       </c>
       <c r="G47" s="115">
         <f>Fish!D11</f>
-        <v>0.27965573781579067</v>
+        <v>0.27965573781578135</v>
       </c>
       <c r="H47" s="42"/>
       <c r="I47" s="42"/>
@@ -3721,11 +3721,11 @@
       </c>
       <c r="F48" s="109">
         <f>Fish!C12</f>
-        <v>-4.2695223915633629E-2</v>
+        <v>-4.2695223915634073E-2</v>
       </c>
       <c r="G48" s="115">
         <f>Fish!D12</f>
-        <v>7.3137310251506604E-2</v>
+        <v>7.3137310251512822E-2</v>
       </c>
       <c r="H48" s="43"/>
       <c r="I48" s="43"/>
@@ -3773,11 +3773,11 @@
       </c>
       <c r="F50" s="111">
         <f>Fish!C22</f>
-        <v>8.7745223232686131E-2</v>
+        <v>8.7745223232685826E-2</v>
       </c>
       <c r="G50" s="117">
         <f>Fish!D22</f>
-        <v>0.10309217333282318</v>
+        <v>0.10309217333282217</v>
       </c>
       <c r="H50" s="45"/>
       <c r="I50" s="45"/>
@@ -3801,11 +3801,11 @@
       </c>
       <c r="F51" s="112">
         <f>Fish!C23</f>
-        <v>8.8287564119833975E-2</v>
+        <v>8.82875641198336E-2</v>
       </c>
       <c r="G51" s="118">
         <f>Fish!D23</f>
-        <v>9.7593564718067197E-2</v>
+        <v>9.7593564718066045E-2</v>
       </c>
       <c r="H51" s="46"/>
       <c r="I51" s="46"/>
@@ -3827,11 +3827,11 @@
       </c>
       <c r="F52" s="112">
         <f>Fish!C24</f>
-        <v>4.1310825018677791E-2</v>
+        <v>4.131082501867761E-2</v>
       </c>
       <c r="G52" s="118">
         <f>Fish!D24</f>
-        <v>4.4894911686997351E-2</v>
+        <v>4.4894911686997593E-2</v>
       </c>
       <c r="H52" s="46"/>
       <c r="I52" s="46"/>
@@ -3853,11 +3853,11 @@
       </c>
       <c r="F53" s="112">
         <f>Fish!C25</f>
-        <v>7.226500839942547E-2</v>
+        <v>7.2265008399425484E-2</v>
       </c>
       <c r="G53" s="118">
         <f>Fish!D25</f>
-        <v>6.1518913298974097E-2</v>
+        <v>6.1518913298975457E-2</v>
       </c>
       <c r="H53" s="46"/>
       <c r="I53" s="46"/>
@@ -6898,8 +6898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7367,8 +7367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="true" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C13" sqref="C10:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7454,10 +7454,10 @@
         <v>61</v>
       </c>
       <c r="C10" s="18">
-        <v>0.17072752641725361</v>
+        <v>0.17072752641725716</v>
       </c>
       <c r="D10" s="18">
-        <v>0.027781796293067068</v>
+        <v>0.027781796293072397</v>
       </c>
       <c r="E10" s="18">
         <v>0.17393061946984731</v>
@@ -7472,10 +7472,10 @@
         <v>62</v>
       </c>
       <c r="C11" s="18">
-        <v>0.34537448398886766</v>
+        <v>0.34537448398886883</v>
       </c>
       <c r="D11" s="18">
-        <v>0.27965573781578135</v>
+        <v>0.2796557378157809</v>
       </c>
       <c r="E11" s="18">
         <v>0.49597818331189858</v>
@@ -7490,10 +7490,10 @@
         <v>63</v>
       </c>
       <c r="C12" s="18">
-        <v>-0.042695223915634073</v>
+        <v>-0.042695223915634573</v>
       </c>
       <c r="D12" s="18">
-        <v>0.073137310251512822</v>
+        <v>0.073137310251511045</v>
       </c>
       <c r="E12" s="18">
         <v>0.031023585864751957</v>
@@ -7508,10 +7508,10 @@
         <v>64</v>
       </c>
       <c r="C13" s="18">
-        <v>0.52659321350951149</v>
+        <v>0.52659321350950927</v>
       </c>
       <c r="D13" s="18">
-        <v>0.61942515563964129</v>
+        <v>0.61942515563963951</v>
       </c>
       <c r="E13" s="18">
         <v>0.29906761135350113</v>
@@ -7526,10 +7526,10 @@
         <v>59</v>
       </c>
       <c r="C14" s="14">
-        <v>1.8092917424992301</v>
+        <v>1.809291742499239</v>
       </c>
       <c r="D14" s="14">
-        <v>1.716711144133658</v>
+        <v>1.7167111441336615</v>
       </c>
       <c r="E14" s="14">
         <v>2.0769209882119757</v>
@@ -7588,10 +7588,10 @@
         <v>61</v>
       </c>
       <c r="C22" s="19">
-        <v>0.087745223232685826</v>
+        <v>0.087745223232686118</v>
       </c>
       <c r="D22" s="19">
-        <v>0.10309217333282217</v>
+        <v>0.10309217333282125</v>
       </c>
       <c r="E22" s="19">
         <v>0.11976329294262</v>
@@ -7602,10 +7602,10 @@
         <v>62</v>
       </c>
       <c r="C23" s="19">
-        <v>0.0882875641198336</v>
+        <v>0.088287564119834128</v>
       </c>
       <c r="D23" s="19">
-        <v>0.097593564718066045</v>
+        <v>0.097593564718065323</v>
       </c>
       <c r="E23" s="19">
         <v>0.1785079900871287</v>
@@ -7616,10 +7616,10 @@
         <v>63</v>
       </c>
       <c r="C24" s="19">
-        <v>0.04131082501867761</v>
+        <v>0.041310825018677728</v>
       </c>
       <c r="D24" s="19">
-        <v>0.044894911686997593</v>
+        <v>0.044894911686997434</v>
       </c>
       <c r="E24" s="19">
         <v>0.15453056276912325</v>
@@ -7630,10 +7630,10 @@
         <v>64</v>
       </c>
       <c r="C25" s="19">
-        <v>0.072265008399425484</v>
+        <v>0.072265008399425512</v>
       </c>
       <c r="D25" s="19">
-        <v>0.061518913298975457</v>
+        <v>0.061518913298973653</v>
       </c>
       <c r="E25" s="19">
         <v>0.21660166504423975</v>
@@ -7644,10 +7644,10 @@
         <v>59</v>
       </c>
       <c r="C26">
-        <v>0.20201988981837624</v>
+        <v>0.20201988981837732</v>
       </c>
       <c r="D26">
-        <v>0.17037139816909169</v>
+        <v>0.17037139816908764</v>
       </c>
       <c r="E26">
         <v>0.39848951125761112</v>
@@ -7726,7 +7726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -7769,19 +7769,19 @@
       <c r="F1" s="23"/>
     </row>
     <row r="2">
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="5" t="s">
         <v>153</v>
       </c>
       <c r="H2" t="s">
@@ -7789,7 +7789,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C3" s="24">
@@ -7810,23 +7810,23 @@
       <c r="H3" s="24"/>
     </row>
     <row r="4">
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>1.5509693622589111</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>1.02196204662323</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>0.22800178825855255</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="5">
         <v>3.7429747581481934</v>
       </c>
-      <c r="G4">
-        <v>8.6819246411323547E-2</v>
+      <c r="G4" s="5">
+        <v>0.086819246411323547</v>
       </c>
       <c r="H4"/>
     </row>
@@ -7841,13 +7841,13 @@
     </row>
     <row r="8">
       <c r="B8"/>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>152</v>
       </c>
       <c r="F8" t="s">
@@ -7863,13 +7863,13 @@
     </row>
     <row r="9">
       <c r="B9"/>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>60</v>
       </c>
       <c r="F9" t="s">
@@ -7884,17 +7884,17 @@
       <c r="K9" s="26"/>
     </row>
     <row r="10">
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C10" s="18">
-        <v>9.7356770042990676E-2</v>
+        <v>0.097356770042985347</v>
       </c>
       <c r="D10" s="18">
-        <v>4.4205479185325233E-2</v>
+        <v>0.044205479185323644</v>
       </c>
       <c r="E10" s="25">
-        <v>3.1137593480004583E-2</v>
+        <v>0.031137593480007671</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
@@ -7904,17 +7904,17 @@
       <c r="M10" s="16"/>
     </row>
     <row r="11">
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="18">
-        <v>0.1989675747992834</v>
+        <v>0.19896757479926919</v>
       </c>
       <c r="D11" s="18">
-        <v>9.9290051197500256E-2</v>
+        <v>0.099290051197501811</v>
       </c>
       <c r="E11" s="25">
-        <v>4.9187881200225603E-2</v>
+        <v>0.049187881200244754</v>
       </c>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
@@ -7924,17 +7924,17 @@
       <c r="M11" s="16"/>
     </row>
     <row r="12">
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C12" s="18">
-        <v>0.25540457621296753</v>
+        <v>0.25540457621295687</v>
       </c>
       <c r="D12" s="18">
-        <v>6.7566533978513407E-2</v>
+        <v>0.067566533978513074</v>
       </c>
       <c r="E12" s="25">
-        <v>3.39593092126879E-4</v>
+        <v>0.00033959309212703485</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25"/>
@@ -7944,17 +7944,17 @@
       <c r="M12" s="16"/>
     </row>
     <row r="13">
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C13" s="18">
-        <v>0.44827107894474594</v>
+        <v>0.44827107894477436</v>
       </c>
       <c r="D13" s="18">
-        <v>8.5840441299547016E-2</v>
+        <v>0.085840441299549611</v>
       </c>
       <c r="E13" s="25">
-        <v>1.9345683718173434E-6</v>
+        <v>1.9345683718160733e-006</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
@@ -7964,17 +7964,17 @@
       <c r="M13" s="16"/>
     </row>
     <row r="14">
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>59</v>
       </c>
       <c r="C14" s="18">
-        <v>4.0232739082393891</v>
+        <v>4.0232739082392754</v>
       </c>
       <c r="D14" s="18">
-        <v>0.89953018228774628</v>
+        <v>0.89953018228774717</v>
       </c>
       <c r="E14" s="25">
-        <v>3.1184638777047287E-5</v>
+        <v>3.1184638777061849e-005</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
@@ -7996,45 +7996,45 @@
     </row>
     <row r="20" ht="18.75" customHeight="true">
       <c r="B20"/>
-      <c r="C20" t="s">
+      <c r="C20" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="5" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="21" ht="18.75" customHeight="true">
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5">
         <v>0.1027066964985659</v>
       </c>
-      <c r="G21"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" ht="18.75" customHeight="true">
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22">
-        <v>1.4046106199844404E-2</v>
-      </c>
-      <c r="G22"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5">
+        <v>0.014046106199844404</v>
+      </c>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" ht="18.75" customHeight="true"/>
     <row r="24" ht="18.75" customHeight="true"/>
@@ -8047,7 +8047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>